<commit_message>
Added features to application
</commit_message>
<xml_diff>
--- a/data/Zbiorcze statystyki.xlsx
+++ b/data/Zbiorcze statystyki.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>a</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>por</t>
+  </si>
+  <si>
+    <t>gertest</t>
   </si>
 </sst>
 </file>
@@ -216,670 +219,6 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pol</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Arkusz1!$B$1:$AB$1</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>a</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>b</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>c</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>d</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>e</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>f</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>g</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>h</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>i</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>j</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>l</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>m</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>o</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>p</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>r</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>s</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>t</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>u</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>v</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>w</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>x</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>inny znak</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$2:$AB$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>8.5849030575285994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.79828416733875</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.16340167292367</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.3424868678554698</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.5726761520705299</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.128169892797552</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.47192655979496</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.13423764589403</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.1147975819310005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0094125827797802</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.2877313176418101</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.10557530869217</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.3163426343327198</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.96003115806114</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.9850781740668699</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.6902495643733002</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>6.6706156711439799E-5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.0351469225239498</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.2745752231403298</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.4533082306170502</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.1375355792376798</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.8662734857693099E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.0687622976422197</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.7038596487044298E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.9173477363333702</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.1084653888098801</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.2537862461117104</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ita</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$3:$AB$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>11.1905069331172</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.02412250508997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.3854717296930801</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.8543777221341999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.926274083762999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0915457162806299</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.9553899515263999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1982512901653599</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.678567704532499</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.89846501101485E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0285397941023599E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.3563034481775098</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.8162445326668601</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.8602763571062999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9.2747697845954509</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.7655762359010301</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.60180156115661998</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.4298094624689996</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.2893908302575801</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6.0209335838634299</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.2636031226934201</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.8783239537847001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.7779814524836301E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.1722590405574399E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.34590356717104E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.67320614100559295</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.36802369443933097</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>cze</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$4:$AB$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>7.3112117865521302</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7645938929498699</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.2313453441115798</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.7584928705777898</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.3554023949813505</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14333429603082901</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.111809913416947</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.8019270968593699</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.5115057287353704</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.3354808771276701</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.5701529959793801</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.85872845327403</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.3800597615068102</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.8496372026077896</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.8942396013395104</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.9035134400759199</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9227425956602197E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.9434455887358801</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.6256471820257197</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.1529540117992303</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.9128509527188902</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.94491946906258</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.8182216917598699E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6.1151068912336497E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.0861642700893599</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.9894035871801099</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13.4996545324964</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>eng</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$5:$AB$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>7.9891600923761397</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.50084378905989</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6394013926064299</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.3231442136057101</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.5573578860502</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2766749212211099</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0858172450121599</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.0441353840745302</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.85030709521146</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.162289524203096</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.70484986565838004</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.9251739592366102</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.47992569023633</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.8754341944435904</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.5777347255302798</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.82644117625883</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.111207365249284</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.0639365681803801</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.2016904554277996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.12610672202781</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.8824970453893601</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.95691698347134801</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.2192117626174199</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.17106632282470299</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.9558222058169801</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.2398044397619505E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.40045536981251301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>fra</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$6:$AB$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>7.8477785916881304</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.96974855351348299</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.9706225500227399</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.7275351353700401</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.724273169441201</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0853031341124</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.03887672163348</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98157564650023699</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.1650599867694096</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.607457889115391</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.3021107518562797E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.4744676816529001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.9406452529765299</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.0276800264709101</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.48979201282798</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.7962297504058</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.1021843758445999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.6763991234735496</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.9187559249779396</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.0778578778617502</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.08973930296857</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.7096024284267</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.116422448261397</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.39734103867289999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.38825728830464901</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.17172629555382499</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.4416466856349399</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
@@ -995,22 +334,22 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:idx val="7"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$8</c:f>
+              <c:f>Arkusz1!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>por</c:v>
+                  <c:v>gertest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
+              <a:schemeClr val="accent2">
                 <a:lumMod val="60000"/>
               </a:schemeClr>
             </a:solidFill>
@@ -1022,90 +361,90 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$B$8:$AB$8</c:f>
+              <c:f>Arkusz1!$B$9:$AB$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>13.52664641</c:v>
+                  <c:v>5.3795443440000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95987774800000003</c:v>
+                  <c:v>2.0742391601869201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.350992148</c:v>
+                  <c:v>3.1121438239999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9385385089999998</c:v>
+                  <c:v>5.3182782309999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.584088270000001</c:v>
+                  <c:v>17.269059240000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.052829612</c:v>
+                  <c:v>1.5622353360000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2340602919999999</c:v>
+                  <c:v>3.0529790299999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4786088909999999</c:v>
+                  <c:v>5.0284605390000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7995888280000001</c:v>
+                  <c:v>7.7750733930000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.31878543999999998</c:v>
+                  <c:v>0.23400694</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1493187E-2</c:v>
+                  <c:v>1.2109684430000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0027183110000002</c:v>
+                  <c:v>3.6773775070000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.6245948349999999</c:v>
+                  <c:v>2.4658827040000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.7535510350000001</c:v>
+                  <c:v>10.515036589999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.78841596</c:v>
+                  <c:v>2.1228234110000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.6271754949999999</c:v>
+                  <c:v>0.57197376799999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2747454709999999</c:v>
+                  <c:v>2.0394836E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6148755030000004</c:v>
+                  <c:v>7.0265603829999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.2997108540000006</c:v>
+                  <c:v>5.9786761899999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.4440281199999996</c:v>
+                  <c:v>5.6919728230000004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.3578640560000004</c:v>
+                  <c:v>3.9152566590000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.592523769</c:v>
+                  <c:v>0.79961130899999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.9453130000000002E-3</c:v>
+                  <c:v>1.663172396</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.22846158599999999</c:v>
+                  <c:v>3.0570718E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.3828758000000003E-2</c:v>
+                  <c:v>5.3975714000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.51923311000000005</c:v>
+                  <c:v>1.1911696519999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.5298184889999999</c:v>
+                  <c:v>2.2585568650000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1121,11 +460,886 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="790222512"/>
-        <c:axId val="790225232"/>
+        <c:axId val="-603064928"/>
+        <c:axId val="-603057856"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>pol</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$1:$AB$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>a</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>b</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>c</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>d</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>e</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>f</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>g</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>h</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>i</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>j</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>k</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>l</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>m</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>n</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>o</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>p</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>q</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>r</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>s</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>t</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>u</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>v</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>w</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>x</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>y</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>z</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>inny znak</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$2:$AB$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>8.5849030575285994</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.79828416733875</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.16340167292367</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.3424868678554698</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7.5726761520705299</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.128169892797552</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.47192655979496</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.13423764589403</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9.1147975819310005</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2.0094125827797802</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3.2877313176418101</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2.10557530869217</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3.3163426343327198</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4.96003115806114</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>6.9850781740668699</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2.6902495643733002</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="0.00E+00">
+                        <c:v>6.6706156711439799E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4.0351469225239498</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4.2745752231403298</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>3.4533082306170502</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2.1375355792376798</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>2.8662734857693099E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>4.0687622976422197</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>5.7038596487044298E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>3.9173477363333702</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>6.1084653888098801</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>9.2537862461117104</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>ita</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$3:$AB$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>11.1905069331172</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.02412250508997</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.3854717296930801</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.8543777221341999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11.926274083762999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.0915457162806299</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.9553899515263999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.1982512901653599</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10.678567704532499</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.89846501101485E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.0285397941023599E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>6.3563034481775098</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2.8162445326668601</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>6.8602763571062999</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>9.2747697845954509</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2.7655762359010301</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.60180156115661998</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>6.4298094624689996</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>5.2893908302575801</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>6.0209335838634299</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>3.2636031226934201</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.8783239537847001</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2.7779814524836301E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>5.1722590405574399E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>1.34590356717104E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.67320614100559295</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.36802369443933097</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>cze</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$4:$AB$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>7.3112117865521302</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.7645938929498699</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.2313453441115798</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.7584928705777898</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8.3554023949813505</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.14333429603082901</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.111809913416947</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2.8019270968593699</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4.5115057287353704</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2.3354808771276701</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3.5701529959793801</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>5.85872845327403</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3.3800597615068102</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>5.8496372026077896</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>7.8942396013395104</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2.9035134400759199</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>3.9227425956602197E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2.9434455887358801</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4.6256471820257197</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>5.1529540117992303</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2.9128509527188902</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>3.94491946906258</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>1.8182216917598699E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>6.1151068912336497E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>2.0861642700893599</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>1.9894035871801099</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>13.4996545324964</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>eng</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$5:$AB$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>7.9891600923761397</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.50084378905989</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.6394013926064299</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.3231442136057101</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>12.5573578860502</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.2766749212211099</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.0858172450121599</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6.0441353840745302</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6.85030709521146</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.162289524203096</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.70484986565838004</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3.9251739592366102</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2.47992569023633</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>6.8754341944435904</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>7.5777347255302798</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>1.82644117625883</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.111207365249284</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>6.0639365681803801</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>6.2016904554277996</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>9.12610672202781</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2.8824970453893601</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.95691698347134801</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2.2192117626174199</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.17106632282470299</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>1.9558222058169801</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>9.2398044397619505E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.40045536981251301</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>fra</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$6:$AB$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>7.8477785916881304</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.96974855351348299</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.9706225500227399</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.7275351353700401</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>14.724273169441201</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.0853031341124</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.03887672163348</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.98157564650023699</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7.1650599867694096</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.607457889115391</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6.3021107518562797E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>5.4744676816529001</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2.9406452529765299</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>7.0276800264709101</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>5.48979201282798</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2.7962297504058</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.1021843758445999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>6.6763991234735496</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>7.9187559249779396</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>7.0778578778617502</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>6.08973930296857</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.7096024284267</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.116422448261397</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.39734103867289999</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.38825728830464901</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.17172629555382499</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>3.4416466856349399</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>por</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$8:$AB$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>13.52664641</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.95987774800000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3.350992148</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.9385385089999998</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>12.584088270000001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.052829612</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.2340602919999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.4786088909999999</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>5.7995888280000001</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.31878543999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.1493187E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3.0027183110000002</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4.6245948349999999</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>4.7535510350000001</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>10.78841596</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2.6271754949999999</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.2747454709999999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>6.6148755030000004</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>8.2997108540000006</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>4.4440281199999996</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>4.3578640560000004</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.592523769</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2.9453130000000002E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.22846158599999999</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>8.3828758000000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.51923311000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>1.5298184889999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="790222512"/>
+        <c:axId val="-603064928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790225232"/>
+        <c:crossAx val="-603057856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1176,7 +1390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="790225232"/>
+        <c:axId val="-603057856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1441,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790222512"/>
+        <c:crossAx val="-603064928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1856,15 +2070,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>168088</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>437029</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:colOff>336176</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2152,23 +2366,13 @@
   <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:AB8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="28" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2857,13 +3061,97 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>5.3795443440000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.0742391601869201</v>
+      </c>
+      <c r="D9">
+        <v>3.1121438239999999</v>
+      </c>
+      <c r="E9">
+        <v>5.3182782309999999</v>
+      </c>
+      <c r="F9">
+        <v>17.269059240000001</v>
+      </c>
+      <c r="G9">
+        <v>1.5622353360000001</v>
+      </c>
+      <c r="H9">
+        <v>3.0529790299999999</v>
+      </c>
+      <c r="I9">
+        <v>5.0284605390000001</v>
+      </c>
+      <c r="J9">
+        <v>7.7750733930000004</v>
+      </c>
+      <c r="K9">
+        <v>0.23400694</v>
+      </c>
+      <c r="L9">
+        <v>1.2109684430000001</v>
+      </c>
+      <c r="M9">
+        <v>3.6773775070000001</v>
+      </c>
+      <c r="N9">
+        <v>2.4658827040000002</v>
+      </c>
+      <c r="O9">
+        <v>10.515036589999999</v>
+      </c>
+      <c r="P9">
+        <v>2.1228234110000002</v>
+      </c>
+      <c r="Q9">
+        <v>0.57197376799999999</v>
+      </c>
+      <c r="R9">
+        <v>2.0394836E-2</v>
+      </c>
+      <c r="S9">
+        <v>7.0265603829999996</v>
+      </c>
+      <c r="T9">
+        <v>5.9786761899999998</v>
+      </c>
+      <c r="U9">
+        <v>5.6919728230000004</v>
+      </c>
+      <c r="V9">
+        <v>3.9152566590000002</v>
+      </c>
+      <c r="W9">
+        <v>0.79961130899999999</v>
+      </c>
+      <c r="X9">
+        <v>1.663172396</v>
+      </c>
+      <c r="Y9">
+        <v>3.0570718E-2</v>
+      </c>
+      <c r="Z9">
+        <v>5.3975714000000001E-2</v>
+      </c>
+      <c r="AA9">
+        <v>1.1911696519999999</v>
+      </c>
+      <c r="AB9">
+        <v>2.2585568650000001</v>
+      </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wszystko zrobione, jeszcze tylko trzeba przeczytać raz sprawko w poszukiwaniu baboli
</commit_message>
<xml_diff>
--- a/data/Zbiorcze statystyki.xlsx
+++ b/data/Zbiorcze statystyki.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
   <si>
     <t>a</t>
   </si>
@@ -116,6 +116,9 @@
     <t>ger</t>
   </si>
   <si>
+    <t>por</t>
+  </si>
+  <si>
     <t>esp</t>
   </si>
   <si>
@@ -126,6 +129,9 @@
   </si>
   <si>
     <t>Dane testowe</t>
+  </si>
+  <si>
+    <t>fra</t>
   </si>
 </sst>
 </file>
@@ -609,330 +615,6 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pol</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Arkusz1!$B$1:$AB$1</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>a</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>b</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>c</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>d</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>e</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>f</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>g</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>h</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>i</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>j</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>l</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>m</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>o</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>p</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>r</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>s</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>t</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>u</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>v</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>w</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>x</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>inny znak</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$2:$AB$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>8.6701363263667499</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7058254254224601</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.26595300158563</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.3550376027720801</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.6166026076788196</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14352438958101599</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4690531786528001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.2279099379359499</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.7854272648358105</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.2097881532942001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.24121760685144</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0184483573993002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.1410683533666002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.0987329385056404</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.9611325053756197</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.6599340487616301</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.3719305743251399E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.1138407529383096</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.2587395656234701</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.3110302488136698</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.2210786117800798</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.31322677898089E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.2612369050292598</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.4643066270821297E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.80048530139686</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.2902898793302704</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.15153853171112</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>eng</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$3:$AB$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>7.9176314664862302</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5112043049538799</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.8924999782224798</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0292872660643102</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.534835659347801</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.4377092557713</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.01287068647936</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.6799011765021099</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.1193152852110204</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.188483684740124</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.68205446959223803</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.0033185565662803</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.4591109677399898</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.9572586388049</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.6973631621490401</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.88260504728394</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.11230360675991399</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.1273145141027801</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.2819452852063504</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.1424078861600595</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.80630515084707</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.0075609811949899</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.0005684067684602</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.186057173908559</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.8139313457674699</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>8.9442869530289904E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.42671317383908902</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
           <c:order val="2"/>
           <c:tx>
@@ -1052,121 +734,6 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ger</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$4:$AB$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>5.35420094414894</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0214554909603</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.2435104878671801</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.1585371260340098</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17.080986429319601</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.55678269793518</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.01449984430577</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.1620607323238703</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.90632473215814</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.21187043411693299</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.2743155542290201</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.7689309160747002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.6217548921662699</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10.3623197841431</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.1654003798371999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.56130297632693404</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.5511255898995401E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7.0995441439303404</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.92322849567757</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.66885849065162</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.7818736941320901</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.80352893111197599</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.6877455529322301</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.3935455026939001E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.1528694395579E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.1778460756768401</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.3021457886186898</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="6"/>
           <c:order val="4"/>
           <c:tx>
@@ -1285,6 +852,236 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$B$7:$AB$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>7.8477785916881304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96974855351348299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9706225500227399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7275351353700401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.724273169441201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0853031341124</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.03887672163348</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98157564650023699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.1650599867694096</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.607457889115391</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.3021107518562797E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.4744676816529001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9406452529765299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.0276800264709101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.48979201282798</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7962297504058</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1021843758445999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6763991234735496</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.9187559249779396</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.0778578778617502</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.08973930296857</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7096024284267</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.116422448261397</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.39734103867289999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.38825728830464901</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.17172629555382499</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.4416466856349399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>por</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$B$8:$AB$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>13.5266464052168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95987774809057602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3509921478347402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9385385091813401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.5840882738894</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0528296115917899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.23406029193181</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4786088912625399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.7995888279444401</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.31878543981936502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1493187397410299E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0027183106213098</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6245948347637498</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7535510350645103</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.7884159616325</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6271754946063002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.27474547059405</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6148755027965196</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.2997108539921491</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.4440281204733099</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3578640563623399</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5925237685573499</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.9453133567498898E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.22846158631791</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.3828757912102203E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.51923310990507299</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.5298184888839399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1297,7 +1094,492 @@
         <c:overlap val="-27"/>
         <c:axId val="-280105408"/>
         <c:axId val="-280096160"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>pol</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$1:$AB$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>a</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>b</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>c</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>d</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>e</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>f</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>g</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>h</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>i</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>j</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>k</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>l</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>m</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>n</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>o</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>p</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>q</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>r</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>s</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>t</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>u</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>v</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>w</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>x</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>y</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>z</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>inny znak</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$2:$AB$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>8.6701363263667499</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.7058254254224601</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.26595300158563</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.3550376027720801</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7.6166026076788196</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.14352438958101599</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.4690531786528001</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.2279099379359499</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8.7854272648358105</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2.2097881532942001</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3.24121760685144</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2.0184483573993002</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3.1410683533666002</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>5.0987329385056404</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>6.9611325053756197</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2.6599340487616301</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.3719305743251399E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4.1138407529383096</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4.2587395656234701</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>3.3110302488136698</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2.2210786117800798</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.31322677898089E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>4.2612369050292598</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>7.4643066270821297E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>3.80048530139686</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>6.2902898793302704</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>9.15153853171112</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>eng</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$3:$AB$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>7.9176314664862302</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.5112043049538799</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.8924999782224798</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.0292872660643102</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>12.534835659347801</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.4377092557713</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.01287068647936</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5.6799011765021099</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7.1193152852110204</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.188483684740124</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.68205446959223803</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>4.0033185565662803</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2.4591109677399898</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>6.9572586388049</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>7.6973631621490401</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>1.88260504728394</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.11230360675991399</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>6.1273145141027801</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>6.2819452852063504</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>9.1424078861600595</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2.80630515084707</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.0075609811949899</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2.0005684067684602</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.186057173908559</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>1.8139313457674699</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>8.9442869530289904E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.42671317383908902</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>ger</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$B$4:$AB$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>5.35420094414894</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.0214554909603</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3.2435104878671801</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.1585371260340098</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>17.080986429319601</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.55678269793518</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3.01449984430577</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5.1620607323238703</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7.90632473215814</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.21187043411693299</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.2743155542290201</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3.7689309160747002</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2.6217548921662699</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>10.3623197841431</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2.1654003798371999</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.56130297632693404</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.5511255898995401E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>7.0995441439303404</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>5.92322849567757</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>5.66885849065162</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>3.7818736941320901</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.80352893111197599</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>1.6877455529322301</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>2.3935455026939001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>5.1528694395579E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>1.1778460756768401</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2.3021457886186898</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="-280105408"/>
@@ -2326,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:AB70"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2960,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>11.237987333023201</v>
@@ -2764,7 +3046,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>11.944947168692799</v>
@@ -2846,6 +3128,178 @@
       </c>
       <c r="AB6">
         <v>2.6168152545795902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>7.8477785916881304</v>
+      </c>
+      <c r="C7">
+        <v>0.96974855351348299</v>
+      </c>
+      <c r="D7">
+        <v>2.9706225500227399</v>
+      </c>
+      <c r="E7">
+        <v>3.7275351353700401</v>
+      </c>
+      <c r="F7">
+        <v>14.724273169441201</v>
+      </c>
+      <c r="G7">
+        <v>1.0853031341124</v>
+      </c>
+      <c r="H7">
+        <v>1.03887672163348</v>
+      </c>
+      <c r="I7">
+        <v>0.98157564650023699</v>
+      </c>
+      <c r="J7">
+        <v>7.1650599867694096</v>
+      </c>
+      <c r="K7">
+        <v>0.607457889115391</v>
+      </c>
+      <c r="L7">
+        <v>6.3021107518562797E-2</v>
+      </c>
+      <c r="M7">
+        <v>5.4744676816529001</v>
+      </c>
+      <c r="N7">
+        <v>2.9406452529765299</v>
+      </c>
+      <c r="O7">
+        <v>7.0276800264709101</v>
+      </c>
+      <c r="P7">
+        <v>5.48979201282798</v>
+      </c>
+      <c r="Q7">
+        <v>2.7962297504058</v>
+      </c>
+      <c r="R7">
+        <v>1.1021843758445999</v>
+      </c>
+      <c r="S7">
+        <v>6.6763991234735496</v>
+      </c>
+      <c r="T7">
+        <v>7.9187559249779396</v>
+      </c>
+      <c r="U7">
+        <v>7.0778578778617502</v>
+      </c>
+      <c r="V7">
+        <v>6.08973930296857</v>
+      </c>
+      <c r="W7">
+        <v>1.7096024284267</v>
+      </c>
+      <c r="X7">
+        <v>0.116422448261397</v>
+      </c>
+      <c r="Y7">
+        <v>0.39734103867289999</v>
+      </c>
+      <c r="Z7">
+        <v>0.38825728830464901</v>
+      </c>
+      <c r="AA7">
+        <v>0.17172629555382499</v>
+      </c>
+      <c r="AB7">
+        <v>3.4416466856349399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>13.5266464052168</v>
+      </c>
+      <c r="C8">
+        <v>0.95987774809057602</v>
+      </c>
+      <c r="D8">
+        <v>3.3509921478347402</v>
+      </c>
+      <c r="E8">
+        <v>4.9385385091813401</v>
+      </c>
+      <c r="F8">
+        <v>12.5840882738894</v>
+      </c>
+      <c r="G8">
+        <v>1.0528296115917899</v>
+      </c>
+      <c r="H8">
+        <v>1.23406029193181</v>
+      </c>
+      <c r="I8">
+        <v>1.4786088912625399</v>
+      </c>
+      <c r="J8">
+        <v>5.7995888279444401</v>
+      </c>
+      <c r="K8">
+        <v>0.31878543981936502</v>
+      </c>
+      <c r="L8">
+        <v>1.1493187397410299E-2</v>
+      </c>
+      <c r="M8">
+        <v>3.0027183106213098</v>
+      </c>
+      <c r="N8">
+        <v>4.6245948347637498</v>
+      </c>
+      <c r="O8">
+        <v>4.7535510350645103</v>
+      </c>
+      <c r="P8">
+        <v>10.7884159616325</v>
+      </c>
+      <c r="Q8">
+        <v>2.6271754946063002</v>
+      </c>
+      <c r="R8">
+        <v>1.27474547059405</v>
+      </c>
+      <c r="S8">
+        <v>6.6148755027965196</v>
+      </c>
+      <c r="T8">
+        <v>8.2997108539921491</v>
+      </c>
+      <c r="U8">
+        <v>4.4440281204733099</v>
+      </c>
+      <c r="V8">
+        <v>4.3578640563623399</v>
+      </c>
+      <c r="W8">
+        <v>1.5925237685573499</v>
+      </c>
+      <c r="X8">
+        <v>2.9453133567498898E-3</v>
+      </c>
+      <c r="Y8">
+        <v>0.22846158631791</v>
+      </c>
+      <c r="Z8">
+        <v>8.3828757912102203E-2</v>
+      </c>
+      <c r="AA8">
+        <v>0.51923310990507299</v>
+      </c>
+      <c r="AB8">
+        <v>1.5298184888839399</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -2857,7 +3311,7 @@
     <row r="56" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -3231,7 +3685,7 @@
     </row>
     <row r="62" spans="1:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B62" s="13">
         <v>11.237987333023201</v>
@@ -3317,7 +3771,7 @@
     </row>
     <row r="63" spans="1:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B63" s="16">
         <v>11.944947168692799</v>
@@ -3403,7 +3857,7 @@
     </row>
     <row r="64" spans="1:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B64" s="20"/>
       <c r="C64" s="20"/>
@@ -3777,7 +4231,7 @@
     </row>
     <row r="69" spans="1:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B69" s="27">
         <v>11.087867979415901</v>
@@ -3863,7 +4317,7 @@
     </row>
     <row r="70" spans="1:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B70" s="16">
         <v>11.98584576</v>

</xml_diff>